<commit_message>
Organized Helpers and memos
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Norbi\Development\Exin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Norbi\Development\Exin\Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="152">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -483,6 +483,9 @@
   </si>
   <si>
     <t>Csináljon biztonsági mentést, mondjuk naponta</t>
+  </si>
+  <si>
+    <t>Alternate row colors in ListViews</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,12 +541,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -557,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -582,9 +579,6 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K90"/>
+  <dimension ref="B1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,20 +2356,24 @@
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="2:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="24" t="s">
+    <row r="83" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C83" s="25">
+      <c r="C83" s="15">
         <v>42119</v>
       </c>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="25"/>
-      <c r="H83" s="26" t="s">
+      <c r="D83" s="15">
+        <v>42156</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83" s="15"/>
+      <c r="H83" s="16" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2481,6 +2479,20 @@
       </c>
       <c r="H90" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" s="1">
+        <v>42157</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H91" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Helpers: Added config transform info (SlowCheetah)
(and trivia)
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="155">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -486,6 +486,15 @@
   </si>
   <si>
     <t>Alternate row colors in ListViews</t>
+  </si>
+  <si>
+    <t>Template based solution for: FileRepoDeveloper</t>
+  </si>
+  <si>
+    <t>Rename MsSql connStr-s</t>
+  </si>
+  <si>
+    <t>They were here earlier, so they have the "default" names (eg ExinConnectionString), but it's misleading. (so eg shoud be ExinMsConnectionString)</t>
   </si>
 </sst>
 </file>
@@ -883,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K91"/>
+  <dimension ref="B1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+      <selection activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,7 +2334,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>19</v>
       </c>
@@ -2342,7 +2351,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>14</v>
       </c>
@@ -2356,7 +2365,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
         <v>14</v>
       </c>
@@ -2377,7 +2386,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
         <v>17</v>
       </c>
@@ -2394,7 +2403,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
         <v>17</v>
       </c>
@@ -2408,7 +2417,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
         <v>17</v>
       </c>
@@ -2422,7 +2431,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>17</v>
       </c>
@@ -2436,7 +2445,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
         <v>17</v>
       </c>
@@ -2453,7 +2462,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
         <v>17</v>
       </c>
@@ -2467,7 +2476,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
         <v>17</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
         <v>23</v>
       </c>
@@ -2493,6 +2502,37 @@
       </c>
       <c r="H91" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B92" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="1">
+        <v>42158</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" s="1">
+        <v>42158</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H93" t="s">
+        <v>153</v>
+      </c>
+      <c r="J93" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TransactionItem (EI,II) default value: Fixed circular dependency with Dependency Injection
UiModels are in Common.dll, DAL.dll referes and uses them; but they also
need to reach some DAL classes (Managers contain the default values, which
maybe can be changed runtime in the future).
So, instead of refactoring the whole, and pulling the UiModels down into
DAL.dll (which could be done, but I would not like to do it); applied DI
for providing default values.

(Also done: Minor NameSpace refactor: WPF.Models->ViewModels)

NOTE: The DefaultValueProvider is initiated in static initializers (in eg
DAL..UnitManager). We should make it sure these get called before using
the things these should initialize first...
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -15,12 +15,12 @@
     <sheet name="todo" sheetId="4" r:id="rId1"/>
     <sheet name="Kategóriák" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="159">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t>Fill with sandbox data: Solution/Repository/FileRepoDeveloper.template/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + DefaultValueProvider.cs</t>
   </si>
 </sst>
 </file>
@@ -903,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,6 +1205,9 @@
       <c r="G19" s="5"/>
       <c r="H19" s="6" t="s">
         <v>16</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
BugFix: Regression ( [Serializable] ) (rollback)
The modified Category and Unit classes weren't marked as Serializable, so
the BinaryFormatter serializer failed. Replaced it with Json.NET
serialization; because we will need that later any case.
Realized the app does not work with it yet, so restored the original
binary formatter solution (and marked the above classes as Serializable)
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="162">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -510,6 +510,12 @@
   </si>
   <si>
     <t>ExportToXlsx</t>
+  </si>
+  <si>
+    <t>ExinConnectionString gets recalculated on every connection opening. Do a static caching</t>
+  </si>
+  <si>
+    <t>DeepClone method works with binary formatter. It haven't worked with json serialization. Solve this, we will need json serialization later</t>
   </si>
 </sst>
 </file>
@@ -907,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K97"/>
+  <dimension ref="B1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,6 +2613,34 @@
       </c>
       <c r="H97" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C98" s="1">
+        <v>42163</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H98" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="1">
+        <v>42163</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H99" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BugFix: Log4net + UnhandledExceptionHandler
* Implemented unhandled exception handler (for WPF)
** Prompts the user before exiting
* Fixed: Log4net object renderer was pointed to UtilsLocal (old project) in config
* Added new Log4net layout pattern
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="163">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -516,6 +516,9 @@
   </si>
   <si>
     <t>DeepClone method works with binary formatter. It haven't worked with json serialization. Solve this, we will need json serialization later</t>
+  </si>
+  <si>
+    <t>MonthlyExpenses: if reordered a column, and click Again, the arraw at header remains, but the new list won't be reordered due to it</t>
   </si>
 </sst>
 </file>
@@ -913,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K99"/>
+  <dimension ref="B1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,6 +2644,20 @@
       </c>
       <c r="H99" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="1">
+        <v>42167</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H100" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BugFix for refactor (part 3): The monthly summaries became corrupt in FileRepo
SummaryItemManagerFileRepo.ReplaceSummary has to recalculate the
summaries, because it does monthly summarizing when saving daily expenses;
so the summary argument contains daily summaries
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="164">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>MonthlyExpenses: if reordered a column, and click Again, the arraw at header remains, but the new list won't be reordered due to it</t>
+  </si>
+  <si>
+    <t>Adding expense item with empty Title is possible</t>
   </si>
 </sst>
 </file>
@@ -916,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K100"/>
+  <dimension ref="B1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,6 +2661,20 @@
       </c>
       <c r="H100" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" s="1">
+        <v>42168</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H101" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Helpers (more tests, todos eliminated)
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="169">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -522,6 +522,21 @@
   </si>
   <si>
     <t>Adding expense item with empty Title is possible</t>
+  </si>
+  <si>
+    <t>Eliminate high level dependencies of (high level) DAL managers</t>
+  </si>
+  <si>
+    <t>So, where possibly, there should be used eg ICategoryManagerDao, and not ICategoryManager</t>
+  </si>
+  <si>
+    <t>Optimalization: Check if we really need IList in DAL Manager (eg CategoryManager.GetAll). IEnumerable would be better</t>
+  </si>
+  <si>
+    <t>SummaryEngineBase.SaveData: proper error message</t>
+  </si>
+  <si>
+    <t>Save to-db/to-file log to ui properly</t>
   </si>
 </sst>
 </file>
@@ -919,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K101"/>
+  <dimension ref="B1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,7 +2622,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
         <v>19</v>
       </c>
@@ -2621,7 +2636,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
         <v>101</v>
       </c>
@@ -2635,7 +2650,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
         <v>101</v>
       </c>
@@ -2649,7 +2664,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B100" s="3" t="s">
         <v>15</v>
       </c>
@@ -2663,18 +2678,77 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C101" s="1">
-        <v>42168</v>
+        <v>42167</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H101" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B102" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102" s="1">
+        <v>42167</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H102" t="s">
+        <v>164</v>
+      </c>
+      <c r="J102" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="1">
+        <v>42167</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H103" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B104" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="1">
+        <v>42167</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H104" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" s="1">
+        <v>42167</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H105" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed project ImportDataToDb to TransportData
And roughly all the (not only code) references to it
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="170">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>A GetHashCode() fv-t igazából nem kell meghívni az Equality vizsgálatkor. Amikor belegondoltam, arra gondoltam, hogy az gyorsít, mert ha nem egyezik a 2 objektum hash kódja, akkor úgysem lehetnek azonosak, nem kell végigmenni a "hosszú" összehasonlításon. Viszont a GetHashCode során ugyanezeket a property-ket használja fel a hash kód készítéséhez... és ott még csak nem is áll meg, ha pl már az 1. property eltérő lenne</t>
-  </si>
-  <si>
-    <t>ImportDataToDb -&gt; ExportDataToFileRepo &lt;--- Így megoldható könnyen unit-ok átnevezése + És ekkor clean-elje a db-t, hogy exe-ből enterre futtatható legyen</t>
   </si>
   <si>
     <t>amikor prompt-ol dátumváltáskor, h változások mentése - legyen mégse gomb</t>
@@ -284,9 +281,6 @@
     <t>Help rész, ahol billentyű kombinációk le vannak írva, plusz egyéb képességek; pl mint át lehet rendezni a wpf gridview oszlopokat (én se tudtam, gyári); meg rendezés implementált, stb</t>
   </si>
   <si>
-    <t>Ne merge-gel szúrja be a summary-kat az ImportDataToDb</t>
-  </si>
-  <si>
     <t>BUG6</t>
   </si>
   <si>
@@ -350,9 +344,6 @@
     <t>Első induláskor figyelmeztessen, h sok a piros, de nem kell megijedni tőle</t>
   </si>
   <si>
-    <t>Az importDataToDb -t lehessen paraméterezni h első induláskor írjon ki megnyugtató szöveget</t>
-  </si>
-  <si>
     <t>RepoPaths statikus, nehogy ez is előbb inicalizálódjon, mint kéne… Élesben még nem próbáltam ki</t>
   </si>
   <si>
@@ -497,12 +488,6 @@
     <t>They were here earlier, so they have the "default" names (eg ExinConnectionString), but it's misleading. (so eg shoud be ExinMsConnectionString)</t>
   </si>
   <si>
-    <t>ImportDataToDb should not depend on config files. It should be configurable from code, because we will need that once we will have options opportunity. Or just set the config files before calling it?</t>
-  </si>
-  <si>
-    <t>Static classes should follow the Singleton design pattern instead of being static. Better said, they should expose an Instance static getter; but they should not be singletons. New instances of them, with new configuration should be createable, we need that for ImportDataToDb</t>
-  </si>
-  <si>
     <t>Fill with sandbox data: Solution/Repository/FileRepoDeveloper.template/</t>
   </si>
   <si>
@@ -537,6 +522,24 @@
   </si>
   <si>
     <t>Save to-db/to-file log to ui properly</t>
+  </si>
+  <si>
+    <t>ImportDataToDb -&gt; ExportDataToFileRepo &lt;--- this way, it would be easy to rename eg units + also do a clean on the db, in order to be runnable from exe</t>
+  </si>
+  <si>
+    <t>The project's new name is TransportData</t>
+  </si>
+  <si>
+    <t>Don't use merge in TransportData for adding the summaries</t>
+  </si>
+  <si>
+    <t>The TransportData project should be parametrized, so the first time it should print calming messages. + Also the WPF app should do so</t>
+  </si>
+  <si>
+    <t>TransportData should not depend on config files. It should be configurable from code, because we will need that once we will have options opportunity. Or just set the config files before calling it?</t>
+  </si>
+  <si>
+    <t>Static classes should follow the Singleton design pattern instead of being static. Better said, they should expose an Instance static getter; but they should not be singletons. New instances of them, with new configuration should be createable, we need that for TransportData</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -630,6 +633,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,17 +955,17 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -975,7 +979,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>25</v>
@@ -1122,7 +1126,7 @@
         <v>7</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -1183,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1237,7 +1241,7 @@
         <v>16</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1350,7 +1354,7 @@
         <v>33</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1479,7 +1483,7 @@
         <v>42008</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>26</v>
@@ -1491,7 +1495,7 @@
         <v>46</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1698,23 +1702,30 @@
       </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="2:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="17" t="s">
+    <row r="42" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="15">
         <v>41992</v>
       </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="18"/>
-      <c r="H42" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="J42" s="18"/>
+      <c r="D42" s="15">
+        <v>42181</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="15"/>
+      <c r="H42" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="J42" s="15"/>
     </row>
     <row r="43" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
@@ -1734,7 +1745,7 @@
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1755,7 +1766,7 @@
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1776,7 +1787,7 @@
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1793,14 +1804,14 @@
         <v>31</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="2:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1817,10 +1828,10 @@
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J47" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="J47" s="20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="48" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1841,10 +1852,10 @@
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J48" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="49" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1865,10 +1876,10 @@
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J49" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="J49" s="12" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -1882,7 +1893,7 @@
         <v>9</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J50" s="13"/>
     </row>
@@ -1897,7 +1908,7 @@
         <v>9</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J51" s="13"/>
     </row>
@@ -1919,7 +1930,7 @@
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1936,7 +1947,7 @@
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="6" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1957,10 +1968,10 @@
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1980,13 +1991,13 @@
         <v>26</v>
       </c>
       <c r="G55" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J55" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="H55" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="56" spans="2:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -2003,7 +2014,7 @@
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J56" s="22"/>
     </row>
@@ -2018,7 +2029,7 @@
         <v>28</v>
       </c>
       <c r="H57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J57" s="1"/>
     </row>
@@ -2036,7 +2047,7 @@
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2053,7 +2064,7 @@
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
@@ -2067,7 +2078,7 @@
         <v>9</v>
       </c>
       <c r="H60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -2081,12 +2092,12 @@
         <v>9</v>
       </c>
       <c r="H61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C62" s="1">
         <v>42008</v>
@@ -2095,15 +2106,15 @@
         <v>26</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C63" s="11">
         <v>42010</v>
@@ -2119,7 +2130,7 @@
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -2133,7 +2144,7 @@
         <v>9</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -2146,8 +2157,8 @@
       <c r="F65" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>106</v>
+      <c r="H65" s="24" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -2158,10 +2169,10 @@
         <v>42015</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H66" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2182,7 +2193,7 @@
       </c>
       <c r="G67" s="11"/>
       <c r="H67" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -2196,7 +2207,7 @@
         <v>9</v>
       </c>
       <c r="H68" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -2210,7 +2221,7 @@
         <v>9</v>
       </c>
       <c r="H69" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -2224,7 +2235,7 @@
         <v>9</v>
       </c>
       <c r="H70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -2238,7 +2249,7 @@
         <v>9</v>
       </c>
       <c r="H71" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2255,7 +2266,7 @@
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
@@ -2269,10 +2280,10 @@
         <v>26</v>
       </c>
       <c r="H73" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J73" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2289,7 +2300,7 @@
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -2303,7 +2314,7 @@
         <v>9</v>
       </c>
       <c r="H75" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2320,7 +2331,7 @@
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -2334,7 +2345,7 @@
         <v>9</v>
       </c>
       <c r="H77" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -2348,7 +2359,7 @@
         <v>9</v>
       </c>
       <c r="H78" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -2362,7 +2373,7 @@
         <v>9</v>
       </c>
       <c r="H79" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -2376,7 +2387,7 @@
         <v>9</v>
       </c>
       <c r="H80" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
@@ -2390,10 +2401,10 @@
         <v>28</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H81" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -2407,7 +2418,7 @@
         <v>28</v>
       </c>
       <c r="H82" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2439,7 @@
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2445,7 +2456,7 @@
       </c>
       <c r="G84" s="5"/>
       <c r="H84" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
@@ -2459,7 +2470,7 @@
         <v>26</v>
       </c>
       <c r="H85" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
@@ -2473,7 +2484,7 @@
         <v>28</v>
       </c>
       <c r="H86" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -2487,7 +2498,7 @@
         <v>28</v>
       </c>
       <c r="H87" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="88" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2515,7 @@
       </c>
       <c r="G88" s="5"/>
       <c r="H88" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
@@ -2518,7 +2529,7 @@
         <v>9</v>
       </c>
       <c r="H89" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
@@ -2532,7 +2543,7 @@
         <v>9</v>
       </c>
       <c r="H90" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -2546,7 +2557,7 @@
         <v>9</v>
       </c>
       <c r="H91" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -2560,7 +2571,7 @@
         <v>9</v>
       </c>
       <c r="H92" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -2574,10 +2585,10 @@
         <v>28</v>
       </c>
       <c r="H93" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J93" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -2591,7 +2602,7 @@
         <v>28</v>
       </c>
       <c r="H94" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
@@ -2605,7 +2616,7 @@
         <v>28</v>
       </c>
       <c r="H95" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
@@ -2619,7 +2630,7 @@
         <v>9</v>
       </c>
       <c r="H96" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
@@ -2633,12 +2644,12 @@
         <v>9</v>
       </c>
       <c r="H97" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C98" s="1">
         <v>42163</v>
@@ -2647,12 +2658,12 @@
         <v>28</v>
       </c>
       <c r="H98" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C99" s="1">
         <v>42163</v>
@@ -2661,7 +2672,7 @@
         <v>28</v>
       </c>
       <c r="H99" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
@@ -2675,7 +2686,7 @@
         <v>26</v>
       </c>
       <c r="H100" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
@@ -2689,7 +2700,7 @@
         <v>26</v>
       </c>
       <c r="H101" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
@@ -2703,10 +2714,10 @@
         <v>28</v>
       </c>
       <c r="H102" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="J102" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
@@ -2720,7 +2731,7 @@
         <v>28</v>
       </c>
       <c r="H103" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
@@ -2734,7 +2745,7 @@
         <v>28</v>
       </c>
       <c r="H104" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
@@ -2748,7 +2759,7 @@
         <v>28</v>
       </c>
       <c r="H105" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2769,87 +2780,87 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BugFix: BackgroundTasks don't get awaited on exit
Created static TaskManager class, which delegates Task.Run; and updated a counter on every Task start and end.

Also done:
* Created ExinLogger.LogInfo method
* Moved FileManagerSafe into subfolder
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="177">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -555,6 +555,12 @@
   </si>
   <si>
     <t>Menu is not localized (English only)</t>
+  </si>
+  <si>
+    <t>The app version at commit (3383988c3f5440b451dab9f55ff6dcbe189410e2) can't init its Sqlite db file if the repo does not exists</t>
+  </si>
+  <si>
+    <t>When saving the changes on exit (so the user pressed Alt+F4, the app asked if it want the changes to be saved; the user clicked yes), the closing procedure does not await background tasks</t>
   </si>
 </sst>
 </file>
@@ -953,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K110"/>
+  <dimension ref="B1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,9 +2853,44 @@
         <v>174</v>
       </c>
     </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B111" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" s="1">
+        <v>42246</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H111" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="112" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C112" s="11">
+        <v>42246</v>
+      </c>
+      <c r="D112" s="11">
+        <v>42246</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G112" s="11"/>
+      <c r="H112" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
BugFix: Can't init the Sqlite db file if the repo does not exists
Only if the repo root did exist, but the subfolders not. In this case, the
repo's subdirectory structure was not initialized. In practise, this would
not have been a valid problem; but fixed now
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="178">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -561,6 +561,9 @@
   </si>
   <si>
     <t>When saving the changes on exit (so the user pressed Alt+F4, the app asked if it want the changes to be saved; the user clicked yes), the closing procedure does not await background tasks</t>
+  </si>
+  <si>
+    <t>Only if the repo root does exist, but the subfolders not. In this case, the repo's subdirectory structure was not initialized. In practise, this is not a valid problem</t>
   </si>
 </sst>
 </file>
@@ -961,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2853,18 +2856,28 @@
         <v>174</v>
       </c>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B111" s="3" t="s">
+    <row r="111" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="11">
         <v>42246</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="D111" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F111" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H111" t="s">
+      <c r="G111" s="11"/>
+      <c r="H111" s="12" t="s">
         <v>175</v>
+      </c>
+      <c r="J111" s="12" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="112" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Default button bold + add-new-item labels' width
* The default button is bold
* The Add-new-daily-expense and Add-new-montly-income forms' labels width is fixed (to Grid auto)
* Exin issues.xlsx: Marked some already finished tasks
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="180">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -314,9 +314,6 @@
     <t>Can not reproducate</t>
   </si>
   <si>
-    <t>Can't reproducate</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -564,6 +561,15 @@
   </si>
   <si>
     <t>Only if the repo root does exist, but the subfolders not. In this case, the repo's subdirectory structure was not initialized. In practise, this is not a valid problem</t>
+  </si>
+  <si>
+    <t>Duplicated</t>
+  </si>
+  <si>
+    <t>Can't reproduce anymore</t>
+  </si>
+  <si>
+    <t>Solved another way…</t>
   </si>
 </sst>
 </file>
@@ -964,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="F115" sqref="F115"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:XFD88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>25</v>
@@ -1150,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -1265,7 +1271,7 @@
         <v>16</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1507,7 +1513,7 @@
         <v>42008</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>94</v>
+        <v>178</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>26</v>
@@ -1744,10 +1750,10 @@
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I42" s="16" t="s">
         <v>164</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>165</v>
       </c>
       <c r="J42" s="15"/>
     </row>
@@ -1971,7 +1977,7 @@
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1992,10 +1998,10 @@
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="J54" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="J54" s="16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="55" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2057,20 +2063,24 @@
       </c>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="2:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
+    <row r="58" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C58" s="15">
         <v>41995</v>
       </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8" t="s">
+      <c r="D58" s="15">
+        <v>42252</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F58" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="9" t="s">
+      <c r="G58" s="15"/>
+      <c r="H58" s="16" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2121,7 +2131,7 @@
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C62" s="1">
         <v>42008</v>
@@ -2130,15 +2140,15 @@
         <v>26</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H62" t="s">
         <v>100</v>
-      </c>
-      <c r="H62" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="63" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" s="11">
         <v>42010</v>
@@ -2154,7 +2164,7 @@
       </c>
       <c r="G63" s="11"/>
       <c r="H63" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -2168,7 +2178,7 @@
         <v>9</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -2182,7 +2192,7 @@
         <v>9</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -2196,7 +2206,7 @@
         <v>68</v>
       </c>
       <c r="H66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2217,7 +2227,7 @@
       </c>
       <c r="G67" s="11"/>
       <c r="H67" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -2231,7 +2241,7 @@
         <v>9</v>
       </c>
       <c r="H68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -2245,7 +2255,7 @@
         <v>9</v>
       </c>
       <c r="H69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -2259,7 +2269,7 @@
         <v>9</v>
       </c>
       <c r="H70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -2273,7 +2283,7 @@
         <v>9</v>
       </c>
       <c r="H71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2290,7 +2300,7 @@
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
@@ -2304,10 +2314,10 @@
         <v>26</v>
       </c>
       <c r="H73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2324,7 +2334,7 @@
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -2338,24 +2348,31 @@
         <v>9</v>
       </c>
       <c r="H75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="15">
+        <v>42102</v>
+      </c>
+      <c r="D76" s="15">
+        <v>42252</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="15"/>
+      <c r="H76" s="16" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="76" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C76" s="5">
-        <v>42102</v>
-      </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G76" s="5"/>
-      <c r="H76" s="6" t="s">
-        <v>124</v>
+      <c r="J76" s="16" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -2369,7 +2386,7 @@
         <v>9</v>
       </c>
       <c r="H77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -2383,7 +2400,7 @@
         <v>9</v>
       </c>
       <c r="H78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -2397,7 +2414,7 @@
         <v>9</v>
       </c>
       <c r="H79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -2411,24 +2428,30 @@
         <v>9</v>
       </c>
       <c r="H80" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B81" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="11">
         <v>42119</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="D81" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G81" s="1" t="s">
+      <c r="G81" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H81" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="H81" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -2442,7 +2465,7 @@
         <v>28</v>
       </c>
       <c r="H82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2463,24 +2486,28 @@
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C84" s="15">
         <v>42129</v>
       </c>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5" t="s">
+      <c r="D84" s="15">
+        <v>42252</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F84" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G84" s="5"/>
-      <c r="H84" s="6" t="s">
-        <v>134</v>
+      <c r="G84" s="15"/>
+      <c r="H84" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
@@ -2494,7 +2521,7 @@
         <v>26</v>
       </c>
       <c r="H85" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
@@ -2508,7 +2535,7 @@
         <v>28</v>
       </c>
       <c r="H86" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -2522,24 +2549,28 @@
         <v>28</v>
       </c>
       <c r="H87" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C88" s="15">
         <v>42139</v>
       </c>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5" t="s">
+      <c r="D88" s="15">
+        <v>42252</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F88" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G88" s="5"/>
-      <c r="H88" s="6" t="s">
-        <v>142</v>
+      <c r="G88" s="15"/>
+      <c r="H88" s="16" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
@@ -2553,7 +2584,7 @@
         <v>9</v>
       </c>
       <c r="H89" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
@@ -2567,7 +2598,7 @@
         <v>9</v>
       </c>
       <c r="H90" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -2581,7 +2612,7 @@
         <v>9</v>
       </c>
       <c r="H91" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -2595,7 +2626,7 @@
         <v>9</v>
       </c>
       <c r="H92" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -2609,10 +2640,10 @@
         <v>28</v>
       </c>
       <c r="H93" t="s">
+        <v>149</v>
+      </c>
+      <c r="J93" t="s">
         <v>150</v>
-      </c>
-      <c r="J93" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -2626,7 +2657,7 @@
         <v>28</v>
       </c>
       <c r="H94" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
@@ -2640,7 +2671,7 @@
         <v>28</v>
       </c>
       <c r="H95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
@@ -2654,7 +2685,7 @@
         <v>9</v>
       </c>
       <c r="H96" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
@@ -2668,12 +2699,12 @@
         <v>9</v>
       </c>
       <c r="H97" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C98" s="1">
         <v>42163</v>
@@ -2682,12 +2713,12 @@
         <v>28</v>
       </c>
       <c r="H98" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C99" s="1">
         <v>42163</v>
@@ -2696,7 +2727,7 @@
         <v>28</v>
       </c>
       <c r="H99" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
@@ -2710,7 +2741,7 @@
         <v>26</v>
       </c>
       <c r="H100" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
@@ -2724,7 +2755,7 @@
         <v>26</v>
       </c>
       <c r="H101" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
@@ -2738,10 +2769,10 @@
         <v>28</v>
       </c>
       <c r="H102" t="s">
+        <v>158</v>
+      </c>
+      <c r="J102" t="s">
         <v>159</v>
-      </c>
-      <c r="J102" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
@@ -2755,7 +2786,7 @@
         <v>28</v>
       </c>
       <c r="H103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
@@ -2769,7 +2800,7 @@
         <v>28</v>
       </c>
       <c r="H104" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
@@ -2783,7 +2814,7 @@
         <v>28</v>
       </c>
       <c r="H105" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.25">
@@ -2797,21 +2828,28 @@
         <v>26</v>
       </c>
       <c r="H106" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="107" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C107" s="11">
+        <v>42213</v>
+      </c>
+      <c r="D107" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G107" s="11"/>
+      <c r="H107" s="12" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B107" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C107" s="1">
-        <v>42213</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H107" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
@@ -2825,7 +2863,7 @@
         <v>28</v>
       </c>
       <c r="H108" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
@@ -2839,7 +2877,7 @@
         <v>26</v>
       </c>
       <c r="H109" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.25">
@@ -2853,7 +2891,7 @@
         <v>28</v>
       </c>
       <c r="H110" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2874,10 +2912,10 @@
       </c>
       <c r="G111" s="11"/>
       <c r="H111" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J111" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="112" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2898,7 +2936,7 @@
       </c>
       <c r="G112" s="11"/>
       <c r="H112" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2919,87 +2957,87 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alternate row colors in ListViews
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="181">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>Solved another way…</t>
+  </si>
+  <si>
+    <t>Can't save daily expenses when the statistics files are not created yet. This means probably when no monthly expenses were already created - which is impossible without daily expenses</t>
   </si>
 </sst>
 </file>
@@ -968,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K112"/>
+  <dimension ref="B1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD88"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:XFD91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,17 +2576,24 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B89" s="3" t="s">
+    <row r="89" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89" s="11">
         <v>42139</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H89" t="s">
+      <c r="D89" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G89" s="11"/>
+      <c r="H89" s="12" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2601,17 +2611,24 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
+    <row r="91" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91" s="11">
         <v>42157</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H91" t="s">
+      <c r="D91" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="11"/>
+      <c r="H91" s="12" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2937,6 +2954,20 @@
       <c r="G112" s="11"/>
       <c r="H112" s="12" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" s="1">
+        <v>42252</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H113" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TransportData: Applied the new solution for "ImportDataToDB"
So using the TransportData_Worker for tasks with FromFile ReadMode, instead of the legacy TransportData_FromFile_ToDb class
* Implemented ID-Insert for Unit- and CategoryManager
** IRepoConfiguration.DbInsertId
** The DB Context classes now have own IRepoConfiguration properties
* DeepClone with Newtonsof.Json
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="184">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -573,6 +573,15 @@
   </si>
   <si>
     <t>Can't save daily expenses when the statistics files are not created yet. This means probably when no monthly expenses were already created - which is impossible without daily expenses</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>This problem did not exist. Only Visual Studio tricked me… With "Break when CLR Exception is thrown" --&gt; this was ticked…</t>
+  </si>
+  <si>
+    <t>I've exchanged the code to the JSON.NET based version, and somehow it worked now without any problem</t>
   </si>
 </sst>
 </file>
@@ -973,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91:XFD91"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:XFD99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2733,18 +2742,28 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B99" s="3" t="s">
+    <row r="99" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99" s="11">
         <v>42163</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="D99" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F99" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H99" t="s">
+      <c r="G99" s="11"/>
+      <c r="H99" s="12" t="s">
         <v>155</v>
+      </c>
+      <c r="J99" s="11" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
@@ -2956,18 +2975,28 @@
         <v>175</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="3" t="s">
+    <row r="113" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C113" s="1">
+      <c r="C113" s="11">
         <v>42252</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="D113" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="F113" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H113" t="s">
+      <c r="G113" s="11"/>
+      <c r="H113" s="12" t="s">
         <v>180</v>
+      </c>
+      <c r="J113" s="11" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BugFix: (Minor) Updated SQL scripts
Some changes were not carried on (probably) from branch PatchTo-0_0_3.
* 2 index names
* Unit.DisplayNames is unique

Also added a bug report
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="187">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -583,12 +583,21 @@
   <si>
     <t>I've exchanged the code to the JSON.NET based version, and somehow it worked now without any problem</t>
   </si>
+  <si>
+    <t>More than likely I've done what I've meant with this. TransportData is fininshed, a lot of static classes got this new structure</t>
+  </si>
+  <si>
+    <t>BUG9</t>
+  </si>
+  <si>
+    <t>There were TransactionItems saved with Category 0 (None - non existing category, this should not have happend)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,6 +609,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -650,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -676,6 +692,7 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K113"/>
+  <dimension ref="B1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:XFD99"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,17 +2658,24 @@
         <v>147</v>
       </c>
     </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B92" s="3" t="s">
+    <row r="92" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C92" s="1">
+      <c r="C92" s="11">
         <v>42158</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H92" t="s">
+      <c r="D92" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" s="11"/>
+      <c r="H92" s="12" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2686,18 +2710,28 @@
         <v>167</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B95" s="3" t="s">
+    <row r="95" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95" s="11">
         <v>42158</v>
       </c>
-      <c r="F95" s="1" t="s">
+      <c r="D95" s="11">
+        <v>42252</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F95" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H95" t="s">
+      <c r="G95" s="11"/>
+      <c r="H95" s="12" t="s">
         <v>168</v>
+      </c>
+      <c r="J95" s="11" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
@@ -2997,6 +3031,23 @@
       </c>
       <c r="J113" s="11" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B114" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C114" s="1">
+        <v>42252</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H114" s="25" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FileRepoDeveloper.template: Filled with sandbox data
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="187">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,20 +2679,27 @@
         <v>148</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B93" s="3" t="s">
+    <row r="93" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C93" s="11">
         <v>42158</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="D93" s="11">
+        <v>42253</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F93" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H93" t="s">
+      <c r="G93" s="11"/>
+      <c r="H93" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="J93" t="s">
+      <c r="J93" s="12" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2734,17 +2741,24 @@
         <v>184</v>
       </c>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B96" s="3" t="s">
+    <row r="96" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="11">
         <v>42158</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H96" t="s">
+      <c r="D96" s="11">
+        <v>42253</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" s="11"/>
+      <c r="H96" s="12" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DeepClone rollbacked to memory stream based version
Changing it (turned out back) to work with Newtonsoft.Json brought back an old problem: eg Category 108 can became 101 during the deserialization... That's why the rollback.
NOTE: A disadvantage is that the MemoryStream based solution needs the [Serializable] markings yet
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="190">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -593,10 +593,13 @@
     <t>There were TransactionItems saved with Category 0 (None - non existing category, this should not have happend)</t>
   </si>
   <si>
-    <t>ReOpened</t>
-  </si>
-  <si>
-    <t>Changing (back) the DeepClone method to work with Newtonsoft.Json brought back an old problem: eg Category 108 can became 101 during the serialization</t>
+    <t>Cancelled (ReOpened)</t>
+  </si>
+  <si>
+    <t>Rollbacked it to the MemoryStream based solution</t>
+  </si>
+  <si>
+    <t>Changing (back) the DeepClone method to work with Newtonsoft.Json brought back an old problem: eg Category 108 can became 101 during the deserialization</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -699,9 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,7 +1009,7 @@
   <dimension ref="B1:K115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2830,25 +2830,29 @@
         <v>183</v>
       </c>
     </row>
-    <row r="100" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="26" t="s">
+    <row r="100" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C100" s="27">
+      <c r="C100" s="15">
         <v>42253</v>
       </c>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27" t="s">
+      <c r="D100" s="15">
+        <v>42253</v>
+      </c>
+      <c r="E100" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="F100" s="27" t="s">
+      <c r="F100" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G100" s="27"/>
-      <c r="H100" s="28" t="s">
+      <c r="G100" s="15"/>
+      <c r="H100" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="J100" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="J100" s="27"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">

</xml_diff>

<commit_message>
Validation: Fixed Title's regex
* Adding expense item with empty Title is no more possible.
* It won't alert validation error when first char is like éÉáÁűŰ...

Old and new regex:
.*[a-zA-Z]+.*
^.*[\w-[\d]]+.*$

* Also added BOS and EOS to RegEx_onlyNumbers
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="190">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -500,9 +500,6 @@
     <t>DeepClone method works with binary formatter. It haven't worked with json serialization. Solve this, we will need json serialization later</t>
   </si>
   <si>
-    <t>MonthlyExpenses: if reordered a column, and click Again, the arraw at header remains, but the new list won't be reordered due to it</t>
-  </si>
-  <si>
     <t>Adding expense item with empty Title is possible</t>
   </si>
   <si>
@@ -600,6 +597,9 @@
   </si>
   <si>
     <t>Changing (back) the DeepClone method to work with Newtonsoft.Json brought back an old problem: eg Category 108 can became 101 during the deserialization</t>
+  </si>
+  <si>
+    <t>MonthlyExpenses: if reordered a column, and click Again, the arrow at header remains, but the new list won't be reordered due to it</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:XFD102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1551,7 @@
         <v>42008</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>26</v>
@@ -1788,10 +1788,10 @@
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="I42" s="16" t="s">
         <v>163</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>164</v>
       </c>
       <c r="J42" s="15"/>
     </row>
@@ -2015,7 +2015,7 @@
       </c>
       <c r="G53" s="5"/>
       <c r="H53" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2112,7 +2112,7 @@
         <v>42252</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F58" s="15" t="s">
         <v>26</v>
@@ -2230,7 +2230,7 @@
         <v>9</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -2410,7 +2410,7 @@
         <v>123</v>
       </c>
       <c r="J76" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>28</v>
       </c>
       <c r="H94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2744,10 +2744,10 @@
       </c>
       <c r="G95" s="11"/>
       <c r="H95" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J95" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="96" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2827,7 +2827,7 @@
         <v>155</v>
       </c>
       <c r="J99" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="100" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2841,45 +2841,59 @@
         <v>42253</v>
       </c>
       <c r="E100" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F100" s="15" t="s">
         <v>26</v>
       </c>
       <c r="G100" s="15"/>
       <c r="H100" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="J100" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="101" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="11">
+        <v>42167</v>
+      </c>
+      <c r="D101" s="11">
+        <v>42253</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G101" s="11"/>
+      <c r="H101" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="J100" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B101" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C101" s="1">
+    </row>
+    <row r="102" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" s="11">
         <v>42167</v>
       </c>
-      <c r="F101" s="1" t="s">
+      <c r="D102" s="11">
+        <v>42253</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F102" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H101" t="s">
+      <c r="G102" s="11"/>
+      <c r="H102" s="12" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B102" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C102" s="1">
-        <v>42167</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H102" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
@@ -2893,10 +2907,10 @@
         <v>28</v>
       </c>
       <c r="H103" t="s">
+        <v>157</v>
+      </c>
+      <c r="J103" t="s">
         <v>158</v>
-      </c>
-      <c r="J103" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
@@ -2910,7 +2924,7 @@
         <v>28</v>
       </c>
       <c r="H104" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
@@ -2924,7 +2938,7 @@
         <v>28</v>
       </c>
       <c r="H105" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.25">
@@ -2938,7 +2952,7 @@
         <v>28</v>
       </c>
       <c r="H106" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
@@ -2952,7 +2966,7 @@
         <v>26</v>
       </c>
       <c r="H107" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="108" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2966,14 +2980,14 @@
         <v>42252</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F108" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G108" s="11"/>
       <c r="H108" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
@@ -2987,7 +3001,7 @@
         <v>28</v>
       </c>
       <c r="H109" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.25">
@@ -3001,7 +3015,7 @@
         <v>26</v>
       </c>
       <c r="H110" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.25">
@@ -3015,7 +3029,7 @@
         <v>28</v>
       </c>
       <c r="H111" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3036,10 +3050,10 @@
       </c>
       <c r="G112" s="11"/>
       <c r="H112" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J112" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="113" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3060,7 +3074,7 @@
       </c>
       <c r="G113" s="11"/>
       <c r="H113" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="114" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3074,17 +3088,17 @@
         <v>42252</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F114" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G114" s="11"/>
       <c r="H114" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J114" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="2:10" x14ac:dyDescent="0.25">
@@ -3098,10 +3112,10 @@
         <v>26</v>
       </c>
       <c r="G115" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H115" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="H115" s="25" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Selection summary on UI
Also made the summaries on the GUI to initially look like this:
"Daily summary: ?"
instead of this
"Daily summary: "
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="216">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -346,9 +346,6 @@
     <t>Eltűnt a logolás a rendszerből!</t>
   </si>
   <si>
-    <t>Kijelölést összegezzen (külön mezőbe)</t>
-  </si>
-  <si>
     <t>Mennyiség megadása ne legyen kötelező. Folyton 1 db-ot írok ugye oda, ahol nem foglalkozom a mennyiséggel. Viszont ugye az 1 db az abszolút valid, csomó mindenből 1 db-ot vesz az ember. Szóval, lehetne inkább az, hogy a mennyiség nem kötelező; pl üresen hagyható a doboza</t>
   </si>
   <si>
@@ -674,6 +671,15 @@
   </si>
   <si>
     <t>DB clean: Implement a logic which cleans the DB from statistics with Amount value 0. Those are just garbage. This logic could be run once per year…</t>
+  </si>
+  <si>
+    <t>How to: do xaml better. More code reusing, more separation</t>
+  </si>
+  <si>
+    <t>Do not use the system provided WPF UI classes directly. Inherit all of them! Use the custom classes on the UI! (More control)</t>
+  </si>
+  <si>
+    <t>Summarize selection on UI (into separate field)</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1130,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I2"/>
     </row>
@@ -1139,7 +1145,7 @@
         <v>42253</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>7</v>
@@ -1307,7 +1313,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I12"/>
     </row>
@@ -1361,27 +1367,30 @@
       </c>
       <c r="G15" s="24"/>
       <c r="H15" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+    <row r="16" spans="2:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="11">
         <v>42088</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="25"/>
+      <c r="D16" s="11">
+        <v>42266</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="17" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -1397,7 +1406,7 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I17"/>
     </row>
@@ -1415,7 +1424,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I18"/>
     </row>
@@ -1433,7 +1442,7 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I19"/>
     </row>
@@ -1451,7 +1460,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I20"/>
     </row>
@@ -1469,7 +1478,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I21"/>
     </row>
@@ -1487,7 +1496,7 @@
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -1505,7 +1514,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I23"/>
     </row>
@@ -1523,7 +1532,7 @@
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -1541,7 +1550,7 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I25"/>
     </row>
@@ -1559,7 +1568,7 @@
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I26" s="5"/>
     </row>
@@ -1577,7 +1586,7 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I27"/>
     </row>
@@ -1595,7 +1604,7 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I28"/>
     </row>
@@ -1613,7 +1622,7 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I29"/>
     </row>
@@ -1631,7 +1640,7 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I30"/>
     </row>
@@ -1649,7 +1658,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I31"/>
     </row>
@@ -1667,7 +1676,7 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I32"/>
     </row>
@@ -1685,7 +1694,7 @@
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I33" s="5"/>
     </row>
@@ -1700,17 +1709,17 @@
         <v>42253</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="11"/>
       <c r="H34" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="2:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1730,13 +1739,13 @@
         <v>22</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H35" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="I35" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1753,7 +1762,7 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I36"/>
     </row>
@@ -1771,7 +1780,7 @@
       </c>
       <c r="G37" s="24"/>
       <c r="H37" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I37" s="25"/>
     </row>
@@ -1788,10 +1797,10 @@
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="I38" s="14" t="s">
         <v>204</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="39" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1808,7 +1817,7 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I39"/>
     </row>
@@ -1823,7 +1832,7 @@
         <v>22</v>
       </c>
       <c r="H40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -1837,7 +1846,7 @@
         <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -1851,7 +1860,39 @@
         <v>7</v>
       </c>
       <c r="H42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="4">
+        <v>42266</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="5" t="s">
         <v>213</v>
+      </c>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="1">
+        <v>42266</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -1916,10 +1957,10 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" t="s">
         <v>138</v>
-      </c>
-      <c r="I2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1936,7 +1977,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1987,10 +2028,10 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2077,7 +2118,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2102,7 +2143,7 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -2144,10 +2185,10 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" t="s">
         <v>193</v>
-      </c>
-      <c r="I2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="3" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2220,10 +2261,10 @@
         <v>103</v>
       </c>
       <c r="I5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2247,7 +2288,7 @@
         <v>35</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2267,7 +2308,7 @@
         <v>22</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>38</v>
@@ -2290,7 +2331,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>40</v>
@@ -2315,13 +2356,13 @@
         <v>22</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>83</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2378,10 +2419,10 @@
         <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" t="s">
         <v>188</v>
-      </c>
-      <c r="H2" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2401,7 +2442,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
@@ -2461,27 +2502,27 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2637,7 +2678,7 @@
         <v>23</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J6" s="8"/>
     </row>
@@ -2662,7 +2703,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J7" s="12"/>
     </row>
@@ -2690,7 +2731,7 @@
         <v>48</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2714,7 +2755,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J9" s="8"/>
     </row>
@@ -2789,7 +2830,7 @@
         <v>35</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J12" s="14"/>
     </row>
@@ -2810,7 +2851,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>38</v>
@@ -2835,7 +2876,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>40</v>
@@ -2864,7 +2905,7 @@
         <v>43</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2925,13 +2966,13 @@
         <v>42008</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>39</v>
@@ -2959,7 +3000,7 @@
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2980,7 +3021,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3004,7 +3045,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J21" s="12"/>
     </row>
@@ -3098,7 +3139,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>37</v>
@@ -3121,7 +3162,7 @@
         <v>22</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>41</v>
@@ -3199,7 +3240,7 @@
         <v>54</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3331,10 +3372,10 @@
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="I35" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>144</v>
       </c>
       <c r="J35" s="12"/>
     </row>
@@ -3356,10 +3397,10 @@
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3397,7 +3438,7 @@
         <v>42252</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>22</v>
@@ -3426,7 +3467,7 @@
         <v>22</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>69</v>
@@ -3479,7 +3520,7 @@
         <v>72</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3503,7 +3544,7 @@
         <v>75</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3523,13 +3564,13 @@
         <v>22</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H43" s="14" t="s">
         <v>83</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J43" s="14"/>
     </row>
@@ -3617,7 +3658,7 @@
         <v>89</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J47" s="8"/>
     </row>
@@ -3642,10 +3683,10 @@
         <v>103</v>
       </c>
       <c r="I48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3666,10 +3707,10 @@
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3689,10 +3730,10 @@
         <v>24</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
@@ -3715,7 +3756,7 @@
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3736,7 +3777,7 @@
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -3759,7 +3800,7 @@
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -3782,7 +3823,7 @@
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3803,7 +3844,7 @@
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3824,7 +3865,7 @@
       </c>
       <c r="G56" s="7"/>
       <c r="H56" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3845,10 +3886,10 @@
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I57" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="I57" s="8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="58" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3869,10 +3910,10 @@
       </c>
       <c r="G58" s="7"/>
       <c r="H58" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3893,7 +3934,7 @@
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3914,7 +3955,7 @@
       </c>
       <c r="G60" s="7"/>
       <c r="H60" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
@@ -3937,10 +3978,10 @@
       </c>
       <c r="G61" s="7"/>
       <c r="H61" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3961,7 +4002,7 @@
       </c>
       <c r="G62" s="7"/>
       <c r="H62" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3982,7 +4023,7 @@
       </c>
       <c r="G63" s="7"/>
       <c r="H63" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3996,14 +4037,14 @@
         <v>42252</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4017,14 +4058,14 @@
         <v>42253</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G65" s="7"/>
       <c r="H65" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4045,10 +4086,10 @@
       </c>
       <c r="G66" s="7"/>
       <c r="H66" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4069,7 +4110,7 @@
       </c>
       <c r="G67" s="7"/>
       <c r="H67" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -4083,17 +4124,17 @@
         <v>42252</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G68" s="7"/>
       <c r="H68" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J68" s="8"/>
     </row>
@@ -4115,10 +4156,10 @@
       </c>
       <c r="G69" s="11"/>
       <c r="H69" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J69" s="12"/>
     </row>

</xml_diff>

<commit_message>
Settings.xml-s (2): MainSettings class
Implemented MainSettings class, which parses and validates the MainSettings.xml
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -307,9 +307,6 @@
     <t>WPF datepciker -&gt; stack overflow</t>
   </si>
   <si>
-    <t>Felhasználó kezelés féle: meg lehessen adni több Root könyvtárat is, azokat el lehessen nevezni. Ki lehessen választani, melyiket akarja most használni…</t>
-  </si>
-  <si>
     <t>* Közlekedés</t>
   </si>
   <si>
@@ -680,6 +677,9 @@
   </si>
   <si>
     <t>Summarize selection on UI (into separate field)</t>
+  </si>
+  <si>
+    <t>Felhasználó kezelés féle: meg lehessen adni több Root könyvtárat is, azokat el lehessen nevezni. Ki lehessen választani, melyiket akarja most használni… 1be tudjon írni, többől tudjon olvasni</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I2"/>
     </row>
@@ -1145,7 +1145,7 @@
         <v>42253</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>7</v>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I12"/>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>91</v>
+        <v>215</v>
       </c>
       <c r="I14"/>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="G15" s="24"/>
       <c r="H15" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I15" s="25"/>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I17"/>
     </row>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I18"/>
     </row>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I19" s="25"/>
     </row>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I20"/>
     </row>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I21"/>
     </row>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I23"/>
     </row>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I25"/>
     </row>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I26" s="5"/>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I27"/>
     </row>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I28"/>
     </row>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I29"/>
     </row>
@@ -1640,7 +1640,7 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I30"/>
     </row>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I31"/>
     </row>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I32"/>
     </row>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I33" s="5"/>
     </row>
@@ -1709,17 +1709,17 @@
         <v>42253</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="11"/>
       <c r="H34" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="2:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1739,13 +1739,13 @@
         <v>22</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H35" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="I35" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I36"/>
     </row>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="G37" s="24"/>
       <c r="H37" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I37" s="25"/>
     </row>
@@ -1797,10 +1797,10 @@
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I38" s="14" t="s">
         <v>203</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="39" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I39" s="25"/>
     </row>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I40" s="5"/>
     </row>
@@ -1850,7 +1850,7 @@
         <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,7 @@
         <v>7</v>
       </c>
       <c r="H42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I43" s="5"/>
     </row>
@@ -1896,7 +1896,7 @@
         <v>7</v>
       </c>
       <c r="H44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1961,10 +1961,10 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
         <v>137</v>
-      </c>
-      <c r="I2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2032,10 +2032,10 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2147,7 +2147,7 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -2189,10 +2189,10 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" t="s">
         <v>192</v>
-      </c>
-      <c r="I2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2262,13 +2262,13 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2292,7 +2292,7 @@
         <v>35</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2312,7 +2312,7 @@
         <v>22</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>38</v>
@@ -2335,7 +2335,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>40</v>
@@ -2360,13 +2360,13 @@
         <v>22</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>83</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2423,10 +2423,10 @@
         <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" t="s">
         <v>187</v>
-      </c>
-      <c r="H2" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2446,87 +2446,87 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2682,7 +2682,7 @@
         <v>23</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J6" s="8"/>
     </row>
@@ -2707,7 +2707,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J7" s="12"/>
     </row>
@@ -2735,7 +2735,7 @@
         <v>48</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J9" s="8"/>
     </row>
@@ -2834,7 +2834,7 @@
         <v>35</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J12" s="14"/>
     </row>
@@ -2855,7 +2855,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>38</v>
@@ -2880,7 +2880,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>40</v>
@@ -2909,7 +2909,7 @@
         <v>43</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2970,13 +2970,13 @@
         <v>42008</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>39</v>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J21" s="12"/>
     </row>
@@ -3143,7 +3143,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>37</v>
@@ -3166,7 +3166,7 @@
         <v>22</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>41</v>
@@ -3244,7 +3244,7 @@
         <v>54</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3376,10 +3376,10 @@
       </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I35" s="12" t="s">
         <v>142</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="J35" s="12"/>
     </row>
@@ -3401,10 +3401,10 @@
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3442,7 +3442,7 @@
         <v>42252</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>22</v>
@@ -3471,7 +3471,7 @@
         <v>22</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>69</v>
@@ -3524,7 +3524,7 @@
         <v>72</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3548,7 +3548,7 @@
         <v>75</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3568,13 +3568,13 @@
         <v>22</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H43" s="14" t="s">
         <v>83</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J43" s="14"/>
     </row>
@@ -3662,7 +3662,7 @@
         <v>89</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J47" s="8"/>
     </row>
@@ -3684,13 +3684,13 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3711,10 +3711,10 @@
       </c>
       <c r="G49" s="11"/>
       <c r="H49" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3734,10 +3734,10 @@
         <v>24</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="G53" s="11"/>
       <c r="H53" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="G56" s="7"/>
       <c r="H56" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3890,10 +3890,10 @@
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I57" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="I57" s="8" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="58" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3914,10 +3914,10 @@
       </c>
       <c r="G58" s="7"/>
       <c r="H58" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="G60" s="7"/>
       <c r="H60" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
@@ -3982,10 +3982,10 @@
       </c>
       <c r="G61" s="7"/>
       <c r="H61" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4006,7 +4006,7 @@
       </c>
       <c r="G62" s="7"/>
       <c r="H62" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4027,7 +4027,7 @@
       </c>
       <c r="G63" s="7"/>
       <c r="H63" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4041,14 +4041,14 @@
         <v>42252</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4062,14 +4062,14 @@
         <v>42253</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G65" s="7"/>
       <c r="H65" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4090,10 +4090,10 @@
       </c>
       <c r="G66" s="7"/>
       <c r="H66" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="2:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4114,7 +4114,7 @@
       </c>
       <c r="G67" s="7"/>
       <c r="H67" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -4128,17 +4128,17 @@
         <v>42252</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G68" s="7"/>
       <c r="H68" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J68" s="8"/>
     </row>
@@ -4160,10 +4160,10 @@
       </c>
       <c r="G69" s="11"/>
       <c r="H69" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J69" s="12"/>
     </row>

</xml_diff>

<commit_message>
Settings.xml-s (3): RepoSettings (1): RepoPath refactor
This was previously a static class (because there was only 1 repo).
Now Config.Repo.Paths holds instance corresponding to the old static
class; and so RepoPath class is not static anymore

Also modified Repo.cs file

NOTE: This is a non-working commit! Only separated for the refactor!
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="217">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>Felhasználó kezelés féle: meg lehessen adni több Root könyvtárat is, azokat el lehessen nevezni. Ki lehessen választani, melyiket akarja most használni… 1be tudjon írni, többől tudjon olvasni</t>
+  </si>
+  <si>
+    <t>Multiple repos, 1 for write to, all for read from. Possibility for settings custom formatted rows for the repos, eg underlined, bold, italic, backgroundColor</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,6 +1900,20 @@
       </c>
       <c r="H44" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="1">
+        <v>42267</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Helpers: SQLite vs Check Constraints
cat Helpers\TODO\MS SQL vs Category 0.txt

The problem is not in MS SQL, it does work properly!
There are Check Constraints on the TransactionItem table; one of them gets violated, that is visible on the picture.
The real problem is that the SQLite file does not have these constraints! The tool with which we convert the MS SQL db into SQLite does not convert the Check Constraints!
...
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="221">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -692,6 +692,9 @@
   </si>
   <si>
     <t>A megvalósítás úgy lett, hogy Add a felirat, ha az ActualItem nincs benn a ListView-ban; Copy ha benne van</t>
+  </si>
+  <si>
+    <t>More use of ViewModels; extracting logic from .xaml.cs to ViewModels</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:I23"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,6 +1987,20 @@
       <c r="G47" s="11"/>
       <c r="H47" s="12" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1">
+        <v>42286</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log: Applied new logging system (1)
... in place of the previous ExinLogger usages

Also done:
* Simplified and extended the logging API
* LogData: 3 modes: StringFormat, ResourceManager, DynamicLocalized
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="234">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -731,6 +731,9 @@
   </si>
   <si>
     <t>Float units</t>
+  </si>
+  <si>
+    <t>"See logs" menu item</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,6 +2109,20 @@
       </c>
       <c r="H53" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="1">
+        <v>42357</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log: New logging system (2)
* BugFix: Exception.Data is not logged via Log4Net
* BugFix: TransportData: LogInit was not called

* Different log levels can be set for UiLoggers and LogLoggers
* LogData.PlusData: Cache the serialized version the first time
* Set up logger colors
* Removed the old ExinLogger and it's instruments
* Cleaned up app configs from Log4Net sections (we configure it from code)
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="237">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -734,6 +734,15 @@
   </si>
   <si>
     <t>"See logs" menu item</t>
+  </si>
+  <si>
+    <t>First starting Exin, TransportData process failed; crashed with unhandled exception; but the Exin app behaved like it could work</t>
+  </si>
+  <si>
+    <t>The app was really usable; the TransportData process probably crashed after the sqlite file was successfully created.</t>
+  </si>
+  <si>
+    <t>First starting Exin, TransportData process failed; because I closed the console window. The Exin app, despite this, continued running; until the first sqlite query; and then crashed with an error message like "no such table". It should have been crashed with "TransportData process failed"</t>
   </si>
 </sst>
 </file>
@@ -1137,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,7 +2050,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>14</v>
       </c>
@@ -2055,7 +2064,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>14</v>
       </c>
@@ -2069,7 +2078,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>14</v>
       </c>
@@ -2083,7 +2092,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>19</v>
       </c>
@@ -2097,7 +2106,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>14</v>
       </c>
@@ -2111,7 +2120,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>14</v>
       </c>
@@ -2124,6 +2133,44 @@
       <c r="H54" t="s">
         <v>233</v>
       </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="1">
+        <v>42361</v>
+      </c>
+      <c r="D55" s="1">
+        <v>42361</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" t="s">
+        <v>234</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="1">
+        <v>42361</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" t="s">
+        <v>236</v>
+      </c>
+      <c r="I56" s="1"/>
     </row>
   </sheetData>
   <sortState ref="B2:I38">

</xml_diff>

<commit_message>
Updated Heleprs + Added changelog
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="244">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>TransportData: It shows a Log.Warn when starting a new app, that the Repository is empty. Sure, since we wanted to create a new, empty one :) We should create a CLI flag that tells this tool if the app is starting the first time</t>
+  </si>
+  <si>
+    <t>Comment TextBox is now multilne, Enter inserts a new line into it. Ctrl+Enter activates the default button. Tell the user this at least once, when pressing Enter in that field</t>
   </si>
 </sst>
 </file>
@@ -1172,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,6 +2283,20 @@
       </c>
       <c r="H62" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="1">
+        <v>42463</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upadted Helpers: Added BUG010
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="245">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -769,6 +769,9 @@
   </si>
   <si>
     <t>Comment TextBox is now multilne, Enter inserts a new line into it. Ctrl+Enter activates the default button. Tell the user this at least once, when pressing Enter in that field</t>
+  </si>
+  <si>
+    <t>When changing anything in the app what writes into MainSettings.xml, some properties will be serialized wrong, and cause the app the next time to crash at start!</t>
   </si>
 </sst>
 </file>
@@ -1175,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,6 +2300,23 @@
       </c>
       <c r="H63" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="1">
+        <v>42463</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H64" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BugFix: The app only can be launched from icon
A .bat file from another directory did not work, because the app resolved paths wrong then.
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="246">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -772,6 +772,9 @@
   </si>
   <si>
     <t>When changing anything in the app what writes into MainSettings.xml, some properties will be serialized wrong, and cause the app the next time to crash at start!</t>
+  </si>
+  <si>
+    <t>Make the JS chart safe - If it can't load, that surface should be empty, but the app should start. Once it happened to me that somehow the WebBrowser did not want to find the path to its html file, the app did not start. Tried again and again, since the prev day it worked. After restarting the OS, it worked again</t>
   </si>
 </sst>
 </file>
@@ -1178,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2317,6 +2320,20 @@
       </c>
       <c r="H64" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="1">
+        <v>42473</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H65" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made JS charts safe
If it can't be load, the app won't crash.
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="246">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,6 +2328,12 @@
       </c>
       <c r="C65" s="1">
         <v>42473</v>
+      </c>
+      <c r="D65" s="1">
+        <v>42498</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
BugFix: MainSettings.xml had properties with wrongly serialized values
Namely these...
* RootDir
* Language
* CurrentRepoNames
... properties got their values wrong serialized. Thus, once the xml got overridden from code, the app could not launch anymore, due to the MainSettings.xml became invalid.
</commit_message>
<xml_diff>
--- a/Helpers/Exin issues.xlsx
+++ b/Helpers/Exin issues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="246">
   <si>
     <t>Havi kiadásoknál a gombot alulról vigyük át felülre, mert ott már úgyis foglalt a hely</t>
   </si>
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,6 +2311,12 @@
       </c>
       <c r="C64" s="1">
         <v>42463</v>
+      </c>
+      <c r="D64" s="1">
+        <v>42498</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>22</v>

</xml_diff>